<commit_message>
develop equal to master
</commit_message>
<xml_diff>
--- a/src/Input_data.xlsx
+++ b/src/Input_data.xlsx
@@ -25,7 +25,7 @@
     <sheet name="Fluorescence" sheetId="6" r:id="rId11"/>
     <sheet name="Fluorescence_norm" sheetId="7" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -597,9 +597,6 @@
   </si>
   <si>
     <t>Lae(47,4780833, 8,365)</t>
-  </si>
-  <si>
-    <t>D:\TRuStee\Deliverables\D3.3\S2\subset_0_of_S2B_MSIL2A_20190318T110759_N0211_R137_T29TQE_20190318T140412_resampled.nc</t>
   </si>
   <si>
     <t>sun_zenith</t>
@@ -803,15 +800,9 @@
     <t>MSI_wl</t>
   </si>
   <si>
-    <t>S2_test</t>
-  </si>
-  <si>
     <t>[PREFERRED] path to file with 18 high resolution (0,01nm) MODTRAN transmittance functions (Alternative to providing Esun and Esky)</t>
   </si>
   <si>
-    <t>run1</t>
-  </si>
-  <si>
     <t>..\output</t>
   </si>
   <si>
@@ -831,6 +822,15 @@
   </si>
   <si>
     <t>..\measured\synthetic\wl.dat</t>
+  </si>
+  <si>
+    <t>..\measured\Sentinel-2_sample.nc</t>
+  </si>
+  <si>
+    <t>sample_synthetic</t>
+  </si>
+  <si>
+    <t>sample_S2</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1535,7 @@
         <v>0.4</v>
       </c>
       <c r="G11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>71</v>
@@ -1814,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1853,10 +1853,10 @@
         <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1873,24 +1873,24 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" t="s">
         <v>213</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1898,7 +1898,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
@@ -1909,7 +1909,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="D7" t="s">
         <v>112</v>
@@ -1920,7 +1920,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C8" t="s">
         <v>104</v>
@@ -1934,7 +1934,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
         <v>104</v>
@@ -1948,13 +1948,13 @@
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C10" t="s">
         <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1966,12 +1966,12 @@
         <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1985,10 +1985,10 @@
         <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2002,7 +2002,7 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2016,7 +2016,7 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2030,7 +2030,7 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2082,21 +2082,21 @@
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="10">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2124,7 +2124,7 @@
         <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2177,7 +2177,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2226,44 +2226,44 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38" s="10">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B39" s="10">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2280,7 +2280,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2318,7 +2318,7 @@
         <v>178</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
       <c r="D2" t="s">
         <v>179</v>
@@ -2340,7 +2340,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D4" t="s">
         <v>106</v>
@@ -2351,7 +2351,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="D5" t="s">
         <v>112</v>
@@ -2362,7 +2362,7 @@
         <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
         <v>104</v>
@@ -2376,7 +2376,7 @@
         <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C7" t="s">
         <v>104</v>
@@ -2390,7 +2390,7 @@
         <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C8" t="s">
         <v>105</v>
@@ -2408,7 +2408,7 @@
         <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2424,7 +2424,7 @@
         <v>165</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
         <v>168</v>
@@ -2438,7 +2438,7 @@
         <v>166</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
         <v>169</v>
@@ -2452,7 +2452,7 @@
         <v>164</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
         <v>170</v>
@@ -2466,7 +2466,7 @@
         <v>167</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
         <v>172</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2537,21 +2537,21 @@
       </c>
       <c r="C21" s="10"/>
       <c r="D21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B22" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>187</v>
       </c>
       <c r="D22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2650,25 +2650,25 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D1" t="s">
         <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F1" t="s">
         <v>123</v>
       </c>
       <c r="G1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H1" t="s">
         <v>180</v>
       </c>
       <c r="I1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3139,31 +3139,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3211,18 +3211,18 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" t="s">
         <v>220</v>
-      </c>
-      <c r="D8" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3246,7 +3246,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -3266,7 +3266,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plot from output file, 2019a compatibility
</commit_message>
<xml_diff>
--- a/src/Input_data.xlsx
+++ b/src/Input_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TRuStee\Deliverables\D3.3\demonstrator\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm_projects\demostrator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9762A22-87A5-4392-A3BF-A9DB0431F976}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="2736" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="8" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="252">
   <si>
     <t>wlmin</t>
   </si>
@@ -708,9 +709,6 @@
   </si>
   <si>
     <t>2018-06-27 11:00:00</t>
-  </si>
-  <si>
-    <t>HyPlant2018</t>
   </si>
   <si>
     <t>Information about sensor and wavelength range used for fitting</t>
@@ -815,28 +813,34 @@
     <t>..\input\radiationdata\FLEX-S3_std.atm</t>
   </si>
   <si>
-    <t>..\measured\synthetic\synthetic_original.dat</t>
-  </si>
-  <si>
-    <t>..\measured\synthetic\synthetic_validation.dat</t>
-  </si>
-  <si>
-    <t>..\measured\synthetic\wl.dat</t>
-  </si>
-  <si>
     <t>..\measured\Sentinel-2_sample.nc</t>
   </si>
   <si>
-    <t>sample_synthetic</t>
-  </si>
-  <si>
     <t>sample_S2</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>D:\validation\Hafiz\hafiz_spec.csv</t>
+  </si>
+  <si>
+    <t>D:\validation\Hafiz\hafiz_wl.csv</t>
+  </si>
+  <si>
+    <t>D:\validation\Hafiz\hafiz_val.csv</t>
+  </si>
+  <si>
+    <t>hafiz</t>
+  </si>
+  <si>
+    <t>D:\validation\Hafiz\hafiz_day.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -941,7 +945,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1032,6 +1036,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1067,6 +1088,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1242,11 +1280,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1739,7 +1777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1762,7 +1800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1788,7 +1826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1811,11 +1849,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1853,7 +1891,7 @@
         <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D2" t="s">
         <v>208</v>
@@ -1873,7 +1911,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -1887,7 +1925,7 @@
         <v>212</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D5" t="s">
         <v>213</v>
@@ -1898,7 +1936,7 @@
         <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D6" t="s">
         <v>106</v>
@@ -1909,7 +1947,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D7" t="s">
         <v>112</v>
@@ -1920,7 +1958,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
         <v>104</v>
@@ -1934,7 +1972,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C9" t="s">
         <v>104</v>
@@ -1948,13 +1986,13 @@
         <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" t="s">
         <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1966,12 +2004,12 @@
         <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1985,10 +2023,10 @@
         <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2002,7 +2040,7 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2016,7 +2054,7 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2030,7 +2068,7 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2082,7 +2120,7 @@
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2090,7 +2128,7 @@
         <v>214</v>
       </c>
       <c r="B24" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
         <v>197</v>
@@ -2118,13 +2156,13 @@
         <v>93</v>
       </c>
       <c r="B27" s="10">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2132,7 +2170,7 @@
         <v>94</v>
       </c>
       <c r="B28" s="10">
-        <v>19.7</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
         <v>98</v>
@@ -2146,7 +2184,7 @@
         <v>95</v>
       </c>
       <c r="B29" s="10">
-        <v>223</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
         <v>98</v>
@@ -2213,7 +2251,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="12">
-        <v>50.874699999999997</v>
+        <v>46.017000000000003</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2221,7 +2259,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="12">
-        <v>6.4484570000000003</v>
+        <v>11.032999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2276,7 +2314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2318,7 +2356,7 @@
         <v>178</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D2" t="s">
         <v>179</v>
@@ -2340,7 +2378,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D4" t="s">
         <v>106</v>
@@ -2351,7 +2389,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
         <v>112</v>
@@ -2362,7 +2400,7 @@
         <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" t="s">
         <v>104</v>
@@ -2376,7 +2414,7 @@
         <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C7" t="s">
         <v>104</v>
@@ -2390,7 +2428,7 @@
         <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s">
         <v>105</v>
@@ -2408,7 +2446,7 @@
         <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2627,7 +2665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2650,25 +2688,25 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D1" t="s">
         <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F1" t="s">
         <v>123</v>
       </c>
       <c r="G1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H1" t="s">
         <v>180</v>
       </c>
       <c r="I1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3102,11 +3140,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3213,13 +3251,16 @@
       <c r="A8" t="s">
         <v>219</v>
       </c>
+      <c r="B8" t="s">
+        <v>251</v>
+      </c>
       <c r="D8" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D9" t="s">
         <v>220</v>
@@ -3232,7 +3273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3275,7 +3316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3483,7 +3524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3509,7 +3550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>